<commit_message>
Added inflows interpolate, updated new and edit model functions, refactored maguduza generation, added maguduza sum calculation
</commit_message>
<xml_diff>
--- a/src/assets/downloads/schedule.xlsx
+++ b/src/assets/downloads/schedule.xlsx
@@ -1078,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="12">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="12">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -1216,7 +1216,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -1233,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -1250,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -1267,7 +1267,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -1301,7 +1301,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -1321,7 +1321,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -1395,7 +1395,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -1412,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -1429,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -1446,7 +1446,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -1463,7 +1463,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -1480,7 +1480,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -1497,7 +1497,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -1514,7 +1514,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31">
@@ -1571,7 +1571,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -1605,7 +1605,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
@@ -1622,7 +1622,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -1817,13 +1817,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -2060,7 +2060,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -2134,7 +2134,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -2151,7 +2151,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -2168,7 +2168,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -2185,7 +2185,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -2202,7 +2202,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -2219,7 +2219,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -2236,7 +2236,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -2253,7 +2253,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31">
@@ -2559,13 +2559,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -2697,7 +2697,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -2714,7 +2714,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -2731,7 +2731,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -2748,7 +2748,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -2765,7 +2765,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -2782,7 +2782,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -2802,7 +2802,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -2876,7 +2876,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -2893,7 +2893,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -2910,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -2927,7 +2927,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -2944,7 +2944,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -2961,7 +2961,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -2978,7 +2978,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -2995,7 +2995,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31">
@@ -3052,7 +3052,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -3069,7 +3069,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -3086,7 +3086,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
@@ -3103,7 +3103,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -3298,15 +3298,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <f>Edwaleni!F14</f>
-        <v>44222.68194444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <f>Edwaleni!H14</f>
-        <v>44222.68194444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -3543,7 +3541,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -3563,7 +3561,7 @@
         <v>10</v>
       </c>
       <c r="F30" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
@@ -3580,7 +3578,7 @@
         <v>10</v>
       </c>
       <c r="F31" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G31" s="31"/>
       <c r="H31" s="31"/>
@@ -3597,7 +3595,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G32" s="31">
         <f>SUM(F30:F32)</f>
@@ -3759,7 +3757,7 @@
         <v>10</v>
       </c>
       <c r="F41" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G41" s="31"/>
       <c r="H41" s="31"/>
@@ -3776,7 +3774,7 @@
         <v>10</v>
       </c>
       <c r="F42" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G42" s="31">
         <f>SUM(F41:F42)</f>

</xml_diff>

<commit_message>
Added Model name duplicate error
</commit_message>
<xml_diff>
--- a/src/assets/downloads/schedule.xlsx
+++ b/src/assets/downloads/schedule.xlsx
@@ -1078,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="12">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="12">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -1216,7 +1216,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -1233,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -1250,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -1267,7 +1267,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -1301,7 +1301,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -1321,7 +1321,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -1395,7 +1395,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -1412,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -1429,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -1446,7 +1446,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -1463,7 +1463,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -1480,7 +1480,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -1497,7 +1497,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -1514,7 +1514,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="31">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31">
@@ -1571,7 +1571,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -1605,7 +1605,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
@@ -1622,7 +1622,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="31">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -1817,13 +1817,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -2060,7 +2060,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -2134,7 +2134,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -2151,7 +2151,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -2168,7 +2168,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -2185,7 +2185,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -2202,7 +2202,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -2219,7 +2219,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -2236,7 +2236,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -2253,7 +2253,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="31">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31">
@@ -2559,13 +2559,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44228.15069444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -2697,7 +2697,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -2714,7 +2714,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -2731,7 +2731,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -2748,7 +2748,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -2765,7 +2765,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -2782,7 +2782,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -2802,7 +2802,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -2876,7 +2876,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -2893,7 +2893,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -2910,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -2927,7 +2927,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -2944,7 +2944,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -2961,7 +2961,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
@@ -2978,7 +2978,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -2995,7 +2995,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31">
@@ -3052,7 +3052,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -3069,7 +3069,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
@@ -3086,7 +3086,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
@@ -3103,7 +3103,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="31">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -3298,15 +3298,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <f>Edwaleni!F14</f>
-        <v>44222.68194444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <f>Edwaleni!H14</f>
-        <v>44222.68194444444</v>
+        <v>44305.361805555556</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -3543,7 +3541,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31">
@@ -3563,7 +3561,7 @@
         <v>10</v>
       </c>
       <c r="F30" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
@@ -3580,7 +3578,7 @@
         <v>10</v>
       </c>
       <c r="F31" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G31" s="31"/>
       <c r="H31" s="31"/>
@@ -3597,7 +3595,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G32" s="31">
         <f>SUM(F30:F32)</f>
@@ -3759,7 +3757,7 @@
         <v>10</v>
       </c>
       <c r="F41" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G41" s="31"/>
       <c r="H41" s="31"/>
@@ -3776,7 +3774,7 @@
         <v>10</v>
       </c>
       <c r="F42" s="31">
-        <v>14.6</v>
+        <v>20</v>
       </c>
       <c r="G42" s="31">
         <f>SUM(F41:F42)</f>

</xml_diff>

<commit_message>
Added admin field in user model
</commit_message>
<xml_diff>
--- a/src/assets/downloads/schedule.xlsx
+++ b/src/assets/downloads/schedule.xlsx
@@ -1078,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="12">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="12">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -1817,13 +1817,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -2559,13 +2559,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -3298,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="52">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H14" s="53">
-        <v>44305.361805555556</v>
+        <v>44291.55694444444</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>

</xml_diff>